<commit_message>
Video File Added of all the Season
</commit_message>
<xml_diff>
--- a/dataset/allMatchVideoDetail/2012/2012_2_season_highlights.xlsx
+++ b/dataset/allMatchVideoDetail/2012/2012_2_season_highlights.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,15 +437,20 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>match_number</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>result</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>toss</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>match_link</t>
         </is>
@@ -457,15 +462,20 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Match 1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 8 wickets</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to field</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=9cfbe23261e4487bb38a236600b41858</t>
         </is>
@@ -477,15 +487,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Match 2</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Delhi Daredevils won by 8 wickets</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t xml:space="preserve">Delhi Daredevils, who chose to field </t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=8cfcd9e5abe1420589af2a54e6d4fe94</t>
         </is>
@@ -497,15 +512,20 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>Match 3</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Pune Warriors India won by 28 runs</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to field</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=9a439394e31d49ffaaea1e5646e89e31</t>
         </is>
@@ -517,15 +537,20 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Match 4</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Rajasthan Royals won by 31 runs</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>Kings XI, who chose to field</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=8540054aca0d413480141edf1276bac9</t>
         </is>
@@ -537,15 +562,20 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Match 5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 20 runs</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to field</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=a07be8977f9f40a0a768f75374391293</t>
         </is>
@@ -557,15 +587,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>Match 6</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 74 runs</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to field</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=87e57899b275490b9f6f8c8b3abb6776</t>
         </is>
@@ -577,15 +612,20 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>Match 7</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>Rajasthan Royals won by 22 runs</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders, who chose to field</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=ac3a64c1d1914823b9618a4e5cd8c4f2</t>
         </is>
@@ -597,15 +637,20 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>Match 8</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>Pune Warriors India won by 22 runs</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>Pune Warriors India, who chose to bat</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=24337e321a2343e3939b5120366981ea</t>
         </is>
@@ -617,15 +662,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>Match 9</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 5 wickets</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to bat</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=78ab7061e0f1447dbe2d532384e3bb72</t>
         </is>
@@ -637,15 +687,20 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>Match 10</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 42 runs</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>Royal Challengers Bangalore, who chose to field</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=95887502fcb04ca9ae3c72134a132c60</t>
         </is>
@@ -657,15 +712,20 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Match 11</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 8 wickets</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to field</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=5d05a67f6af247488c4de41e75d0fec3</t>
         </is>
@@ -677,15 +737,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>Match 12</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 27 runs</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to field</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=b930c20d38514dd385bf0be48b32ab0b</t>
         </is>
@@ -697,15 +762,20 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>Match 13</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 5 wickets</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Royal Challengers Bangalore, who chose to bat</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=1a5689f15948461396fa4f8b8af84537</t>
         </is>
@@ -717,15 +787,20 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>Match 14</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 7 wickets</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Kings XI Punjab, who chose to field</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=6ef2464d76bf4bc4ad72cc60c0c7c824</t>
         </is>
@@ -737,15 +812,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>Match 15</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 5 wickets</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to bat</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=886c9ffe516e40b38bd4242e70337a50</t>
         </is>
@@ -757,15 +837,20 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>Match 16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>Pune Warriors India won by 7 wickets</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>Chennai Super Kings, who chose to bat</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=851bc87572294b1591d7663d4fbb8700</t>
         </is>
@@ -777,15 +862,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>Match 17</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 2 runs</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders, who chose to field</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=9b281ea3bf7d4ec48ae1ad290661260b</t>
         </is>
@@ -797,15 +887,20 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>Match 18</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>Rajasthan Royals won by 59 runs</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to bat</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=d336bdc658c84000a6aeb272a2356997</t>
         </is>
@@ -817,15 +912,20 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
+          <t>Match 19</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 7 wickets</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to field</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=bbb8a8efd044478b9517f4963fe8ea95</t>
         </is>
@@ -837,15 +937,20 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>Match 20</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>Rajasthan Royals won by 5 wickets</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to bat</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=019aaa0841f947b1a8f5bc2bdfc787ed</t>
         </is>
@@ -857,15 +962,20 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>Match 21</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 6 wickets</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>Pune Warriors India, who chose to bat</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=e09f6cd1d73143198b96232f61b8d799</t>
         </is>
@@ -877,15 +987,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>Match 22</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 8 wickets</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Kings XI Punjab, who chose to bat</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=f0a73ae27000432289e786cfff251470</t>
         </is>
@@ -897,15 +1012,20 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>Match 23</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 5 wickets</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to bat</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=3322328171de46ccaa792a3026bbd9ff</t>
         </is>
@@ -917,15 +1037,20 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>Match 24</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 13 runs</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>Pune Warriors India, who chose to field</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=6d3b039fd50c487a8f728027017c9bd6</t>
         </is>
@@ -937,15 +1062,20 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>Match 25</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 5 wickets</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Royal Challengers Bangalore, who chose to field</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=a997e577454c45adbb242a47bab1d10b</t>
         </is>
@@ -957,15 +1087,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>Match 26</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 7 wickets</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to bat</t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=52ecdf097e2f4f06a6cf353b919aa784</t>
         </is>
@@ -977,15 +1112,20 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>Match 27</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>Pune Warriors India won by 20 runs</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to field</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=74470b6a51dd45ce808138d8165f088d</t>
         </is>
@@ -997,15 +1137,20 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>Match 28</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 6 wickets</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to bat</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=f61aeccbd8d94263995acc2793f4fd18</t>
         </is>
@@ -1017,15 +1162,20 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>Match 29</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 5 wickets</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders, who chose to field</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=7f0c271361c443c0be86d25f6c360b80</t>
         </is>
@@ -1037,15 +1187,20 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>Match 30</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 46 runs</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to field</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=963ddf3664cd4500a6d03f330b33e222</t>
         </is>
@@ -1057,15 +1212,20 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>Match 31</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>Delhi Daredevils won by 8 wickets</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Pune Warriors, who elected to bat</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=c815358df32447819a52d647f65212e2</t>
         </is>
@@ -1077,15 +1237,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>Match 33</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 4 wickets</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Kings XI Punjab, who chose to bat</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=928f6dacc28f47dca10d7ec47d09619c</t>
         </is>
@@ -1097,15 +1262,20 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>Match 35</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>Deccan Chargers won by 18 runs</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to bat</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=9628fd0671e941fca63f8e4742d4bbb5</t>
         </is>
@@ -1117,15 +1287,20 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>Match 36</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 37 runs</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to field</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=d863ccb42ff6400db422d728de21878f</t>
         </is>
@@ -1137,15 +1312,20 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>Match 37</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 7 runs</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>Kings XI Punjab, who chose to bat</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=057bf050e33844d498a6e827a4b9f726</t>
         </is>
@@ -1157,15 +1337,20 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>Match 38</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 47 runs</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders, who chose to bat</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=20b7a63aaa83409e8bfc46d76e04e79d</t>
         </is>
@@ -1177,15 +1362,20 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>Match 39</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 1 run</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to bat</t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=afe77113dae344a4b8e2d509b33c6c1c</t>
         </is>
@@ -1197,15 +1387,20 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>Match 40</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 5 wickets</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to bowl</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=d60f8c99c6a14e31866685b1266b3b19</t>
         </is>
@@ -1217,15 +1412,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>Match 41</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 5 wickets</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>Chennai Super Kings, who chose to bat</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=b2e6e432d56a42e7b93c8b72c4a499c1</t>
         </is>
@@ -1237,15 +1437,20 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>Match 42</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>Deccan Chargers won by 13 runs</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to bat</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=b6ca972222d54ad0b129b7e063f7137f</t>
         </is>
@@ -1257,15 +1462,20 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>Match 43</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 6 wickets</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>Rajasthan Royals, and chose to bat</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=31e5fa13802040cc84237b3fa783f6bd</t>
         </is>
@@ -1277,15 +1487,20 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>Match 44</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 4 wickets</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Kings XI Punjab, who chose to field</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=f93a374732594fd2a043ceb7de06d4c7</t>
         </is>
@@ -1297,15 +1512,20 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>Match 45</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 1 run</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to bat</t>
         </is>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="E44" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=0dff4e7f030f4018a69386f99acbdd65</t>
         </is>
@@ -1317,15 +1537,20 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>Match 46</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 10 runs</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Chennai Super Kings, who chose to bat</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="E45" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=4ae89282a3b84024bc11ae5b2288f6df</t>
         </is>
@@ -1337,15 +1562,20 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>Match 47</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 7 runs</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders, who chose to bat</t>
         </is>
       </c>
-      <c r="D46" t="inlineStr">
+      <c r="E46" t="inlineStr">
         <is>
           <t xml:space="preserve"> http://iplt20.com/videos?mid=a47fcee0cb7547a48046df25aa40d61e</t>
         </is>
@@ -1357,15 +1587,20 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>Match 48</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>Rajasthan Royals won by 43 runs</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>Rajastan Royals, who chose to bat</t>
         </is>
       </c>
-      <c r="D47" t="inlineStr">
+      <c r="E47" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=53d958be5187423caf272da4274d3db6</t>
         </is>
@@ -1377,15 +1612,20 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>Match 49</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 2 wickets</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to field</t>
         </is>
       </c>
-      <c r="D48" t="inlineStr">
+      <c r="E48" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=5cf7f790e8c94ab3839ead1d15f0666d</t>
         </is>
@@ -1397,15 +1637,20 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>Match 50</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 5 wickets</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>Royal Challengers Bangalore, who chose to field</t>
         </is>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="E49" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=e5d2b0ef385245859afe587e7bbec49a</t>
         </is>
@@ -1417,15 +1662,20 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>Match 51</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 6 wickets</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to bat</t>
         </is>
       </c>
-      <c r="D50" t="inlineStr">
+      <c r="E50" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=1eec0e7b251a4b0d8f84195c35d14aca</t>
         </is>
@@ -1437,15 +1687,20 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>Match 52</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>Rajasthan Royals won by 7 wickets</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>Pune Warriors India, who chose to bat</t>
         </is>
       </c>
-      <c r="D51" t="inlineStr">
+      <c r="E51" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=f52a52d6c6b4498aaa2219fe72174cef</t>
         </is>
@@ -1457,15 +1712,20 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>Match 53</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 25 runs</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to field</t>
         </is>
       </c>
-      <c r="D52" t="inlineStr">
+      <c r="E52" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=27f4f2949b5247eeb3de6312e8236de9</t>
         </is>
@@ -1477,15 +1737,20 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>Match 54</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 9 wickets</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>Royal Challengers Bangalore, who chose to field</t>
         </is>
       </c>
-      <c r="D53" t="inlineStr">
+      <c r="E53" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=14588a5fd41e44b1a2128685c8ebc780</t>
         </is>
@@ -1497,15 +1762,20 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>Match 55</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 9 wickets</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to bat</t>
         </is>
       </c>
-      <c r="D54" t="inlineStr">
+      <c r="E54" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=32d62f4f3e8a4c5daacd8a235d47d41d</t>
         </is>
@@ -1517,15 +1787,20 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>Match 56</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 4 wickets</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>Chennai Super Kings, who chose to field</t>
         </is>
       </c>
-      <c r="D55" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=0922df4b58114cdc86646f3a1fe0ce37</t>
         </is>
@@ -1537,15 +1812,20 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>Match 57</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 35 runs</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>Pune Warriors India, who chose to field</t>
         </is>
       </c>
-      <c r="D56" t="inlineStr">
+      <c r="E56" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos?mid=56609e04ed4545c3935a72574db71a73</t>
         </is>
@@ -1557,15 +1837,20 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>Match 58</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 27 runs</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to bat</t>
         </is>
       </c>
-      <c r="D57" t="inlineStr">
+      <c r="E57" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos/media/id/d10988863f954f6c9fb116c79efa2f28/ipl-2012-match-58-kkr-vs-mi-highlights</t>
         </is>
@@ -1577,15 +1862,20 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>Match 59</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 9 wickets</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>Chennai Super Kings, who chose to field</t>
         </is>
       </c>
-      <c r="D58" t="inlineStr">
+      <c r="E58" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos/media/id/6d987175eab448c6980612f667e88e2b/ipl-2012-match-59-csk-vs-dd-highlights</t>
         </is>
@@ -1597,15 +1887,20 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>Match 60</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>Rajasthan Royals won by 45 runs</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to bat</t>
         </is>
       </c>
-      <c r="D59" t="inlineStr">
+      <c r="E59" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos/media/id/8c3db767742149f0be91a24843e91325/ipl-2012-match-60-rr-vs-pwi-highlights</t>
         </is>
@@ -1617,15 +1912,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>Match 61</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 4 wickets</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>Deccan Chargers, who chose to bat</t>
         </is>
       </c>
-      <c r="D60" t="inlineStr">
+      <c r="E60" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos/media/id/63cec82693c14f5a8d1b29acb47176d7/ipl-2012-match-61-kxip-vs-dc-highlights</t>
         </is>
@@ -1637,15 +1937,20 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>Match 62</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 5 wickets</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to field</t>
         </is>
       </c>
-      <c r="D61" t="inlineStr">
+      <c r="E61" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos/media/id/93d81d6c2e144314ac0ffe3440a44aa9/ipl-2012-match-62-rcb-vs-mi-highlights</t>
         </is>
@@ -1657,15 +1962,20 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
+          <t>Match 63</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 5 wickets</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>Chennai Super Kings, who chose to field</t>
         </is>
       </c>
-      <c r="D62" t="inlineStr">
+      <c r="E62" t="inlineStr">
         <is>
           <t>http://iplt20.com/videos/media/id/55549f6e478141b9ab904798b87069cf/ipl-2012-match-63-kkr-vs-csk-highlights</t>
         </is>
@@ -1677,15 +1987,20 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>Match 64</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 5 wickets</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>Kings XI Punjab, who chose to bat</t>
         </is>
       </c>
-      <c r="D63" t="inlineStr">
+      <c r="E63" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=20edfe74d63648928d0935af3d1fff90</t>
         </is>
@@ -1697,15 +2012,20 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>Match 65</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 32 runs</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to field</t>
         </is>
       </c>
-      <c r="D64" t="inlineStr">
+      <c r="E64" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=bb13babf4c4d4b528f287b683ecfe2c2</t>
         </is>
@@ -1717,15 +2037,20 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>Match 66</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
           <t>Kings XI Punjab won by 6 wickets</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>Kings XI Punjab, who chose to field</t>
         </is>
       </c>
-      <c r="D65" t="inlineStr">
+      <c r="E65" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=2ae42a4b4c124aa2b276bca97d143d8c</t>
         </is>
@@ -1737,15 +2062,20 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>Match 67</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>Royal Challengers Bangalore won by 21 runs</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to field</t>
         </is>
       </c>
-      <c r="D66" t="inlineStr">
+      <c r="E66" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=16d0251db13a44d486e3847d7c053091</t>
         </is>
@@ -1757,15 +2087,20 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>Match 68</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>Deccan Chargers won by 5 wickets</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to bat</t>
         </is>
       </c>
-      <c r="D67" t="inlineStr">
+      <c r="E67" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=2e6d65b63f594f30be4b4e61bcad765e</t>
         </is>
@@ -1777,15 +2112,20 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>Match 69</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>Delhi Capitals won by 6 wickets</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>Delihi Daredevils, who chose to field</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="E68" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=1f6cf26f7c9d4dec83c4a75c13a29086</t>
         </is>
@@ -1797,15 +2137,20 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>Match 70</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 34 runs</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders, who chose to bat</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=1e727f526e4c47229e51226142aa848a</t>
         </is>
@@ -1817,15 +2162,20 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>Match 71</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>Deccan Chargers won by 9 runs</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>Royal Challengers Bangalore, who chose to bowl</t>
         </is>
       </c>
-      <c r="D70" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=99b51939ccb343768389b57207c7584d</t>
         </is>
@@ -1837,15 +2187,20 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
+          <t>Match 72</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>Mumbai Indians won by 10 wickets</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>Rajasthan Royals, who chose to bat</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=993ababa573e4c4ebf4b3c581ac61106</t>
         </is>
@@ -1857,15 +2212,20 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>Qualifier 1</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 18 runs</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>Kolkata Knight Riders, who chose to bat</t>
         </is>
       </c>
-      <c r="D72" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=e989eb0f278e4542bcebecfc4ac90041</t>
         </is>
@@ -1877,15 +2237,20 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>Eliminator</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 38 runs</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>Mumbai Indians, who chose to field</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="E73" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=1236d0aa1e4d430f9c8143939d608b0a</t>
         </is>
@@ -1897,15 +2262,20 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
+          <t>Qualifier 2</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
           <t>Chennai Super Kings won by 86 runs</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>Delhi Daredevils, who chose to bowl</t>
         </is>
       </c>
-      <c r="D74" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=2ad9156e94d549eb8d045a3f26e9568e</t>
         </is>
@@ -1917,15 +2287,20 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
+          <t>Final</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
           <t>Kolkata Knight Riders won by 5 wickets</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>Chennai Super Kings, who chose to bat</t>
         </is>
       </c>
-      <c r="D75" t="inlineStr">
+      <c r="E75" t="inlineStr">
         <is>
           <t>http://www.iplt20.com/videos?mid=aa5bbd78b00d474b814ce7aa3d2cc8c3</t>
         </is>

</xml_diff>